<commit_message>
Unify USB C connector
Unified USB-C Connection
Reliability issues present with type C pogo pin board
</commit_message>
<xml_diff>
--- a/HW/Production/GC-Ultimate PCB Notes.xlsx
+++ b/HW/Production/GC-Ultimate PCB Notes.xlsx
@@ -5,8 +5,7 @@
   <sheets>
     <sheet state="visible" name="Main PCB BOM" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="SubStick PCB BOM" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="USBC BOM" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="PCB Production Notes" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="PCB Production Notes" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="165">
   <si>
     <t>#</t>
   </si>
@@ -40,7 +39,7 @@
     <t>B1</t>
   </si>
   <si>
-    <t>Battery</t>
+    <t>Battery Connector</t>
   </si>
   <si>
     <t>Connector_JST:JST_PH_B2B-PH-K_1x02_P2.00mm_Vertical</t>
@@ -154,16 +153,13 @@
     <t>Fuse:Fuse_1206_3216Metric_Pad1.42x1.75mm_HandSolder</t>
   </si>
   <si>
-    <t>J5, J6, J7, J8, J9, J10, J11, J12</t>
-  </si>
-  <si>
-    <t>Conn_01x01_Pin</t>
-  </si>
-  <si>
-    <t>hhl:YZ72015053P-01</t>
-  </si>
-  <si>
-    <t>YZ72015053P-01</t>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>UJ31-CH-G1-SMT-TR</t>
+  </si>
+  <si>
+    <t>hhl:CUI_UJ31-CH-G1-SMT-TR</t>
   </si>
   <si>
     <t>J13</t>
@@ -175,15 +171,6 @@
     <t>hhl:5034800640</t>
   </si>
   <si>
-    <t>J14</t>
-  </si>
-  <si>
-    <t>USB4105-GF-A-060</t>
-  </si>
-  <si>
-    <t>hhl:GCT_USB4105-GF-A-060</t>
-  </si>
-  <si>
     <t>L1, L2, L3, L4</t>
   </si>
   <si>
@@ -283,7 +270,7 @@
     <t>R21, R22</t>
   </si>
   <si>
-    <t>5.1k</t>
+    <t>5.1kohm</t>
   </si>
   <si>
     <t>R32, R35</t>
@@ -466,18 +453,6 @@
     <t>U1, U2</t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>UJ31-CH-G1-SMT-TR</t>
-  </si>
-  <si>
-    <t>hhl:CUI_UJ31-CH-G1-SMT-TR</t>
-  </si>
-  <si>
-    <t>5.1kohm</t>
-  </si>
-  <si>
     <t>Main</t>
   </si>
   <si>
@@ -485,9 +460,6 @@
   </si>
   <si>
     <t>Trigger</t>
-  </si>
-  <si>
-    <t>USBC</t>
   </si>
   <si>
     <t>Layers</t>
@@ -584,12 +556,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -620,10 +595,6 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -1084,6 +1055,9 @@
       <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F10" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11">
@@ -1208,7 +1182,7 @@
         <v>46</v>
       </c>
       <c r="C17" s="1">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>47</v>
@@ -1217,7 +1191,7 @@
         <v>48</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -1226,19 +1200,19 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -1247,19 +1221,19 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -1268,19 +1242,19 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="H20" s="1"/>
     </row>
@@ -1292,7 +1266,7 @@
         <v>59</v>
       </c>
       <c r="C21" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>60</v>
@@ -1301,7 +1275,7 @@
         <v>61</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H21" s="1"/>
     </row>
@@ -1310,16 +1284,16 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>64</v>
@@ -1331,19 +1305,19 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="H23" s="1"/>
     </row>
@@ -1352,19 +1326,19 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="H24" s="1"/>
     </row>
@@ -1373,20 +1347,18 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
     <row r="26">
@@ -1394,16 +1366,16 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>76</v>
+        <v>1.0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>100.0</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1413,13 +1385,13 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C27" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D27" s="1">
-        <v>100.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>77</v>
@@ -1432,16 +1404,16 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="H28" s="1"/>
     </row>
@@ -1450,16 +1422,16 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C29" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>83</v>
+        <v>2.0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>27.0</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H29" s="1"/>
     </row>
@@ -1468,16 +1440,16 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C30" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D30" s="1">
-        <v>27.0</v>
+        <v>330.0</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="H30" s="1"/>
     </row>
@@ -1486,16 +1458,16 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C31" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D31" s="1">
-        <v>330.0</v>
+        <v>0.0</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="H31" s="1"/>
     </row>
@@ -1504,13 +1476,13 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C32" s="1">
         <v>2.0</v>
       </c>
-      <c r="D32" s="1">
-        <v>0.0</v>
+      <c r="D32" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>77</v>
@@ -1522,16 +1494,16 @@
         <v>32.0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C33" s="1">
         <v>2.0</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -1541,18 +1513,20 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C34" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
     <row r="35">
@@ -1563,7 +1537,7 @@
         <v>92</v>
       </c>
       <c r="C35" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>93</v>
@@ -1583,7 +1557,7 @@
         <v>96</v>
       </c>
       <c r="C36" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>97</v>
@@ -1612,7 +1586,7 @@
         <v>102</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H37" s="1"/>
     </row>
@@ -1621,19 +1595,19 @@
         <v>37.0</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C38" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="G38" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H38" s="1"/>
     </row>
@@ -1642,19 +1616,19 @@
         <v>38.0</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C39" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="40">
@@ -1665,7 +1639,7 @@
         <v>110</v>
       </c>
       <c r="C40" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>111</v>
@@ -1686,7 +1660,7 @@
         <v>114</v>
       </c>
       <c r="C41" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>115</v>
@@ -1728,7 +1702,7 @@
         <v>122</v>
       </c>
       <c r="C43" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>123</v>
@@ -1737,7 +1711,7 @@
         <v>124</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H43" s="1"/>
     </row>
@@ -1746,19 +1720,19 @@
         <v>43.0</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C44" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="G44" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -1767,19 +1741,19 @@
         <v>44.0</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C45" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="G45" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H45" s="1"/>
     </row>
@@ -1788,19 +1762,19 @@
         <v>45.0</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C46" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="G46" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H46" s="1"/>
     </row>
@@ -1809,19 +1783,19 @@
         <v>46.0</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C47" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="H47" s="1"/>
     </row>
@@ -1847,24 +1821,12 @@
       <c r="H48" s="1"/>
     </row>
     <row r="49">
-      <c r="A49" s="1">
-        <v>48.0</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C49" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>145</v>
-      </c>
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="G49" s="1"/>
       <c r="H49" s="1"/>
     </row>
     <row r="50">
@@ -1970,19 +1932,19 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C3" s="1">
         <v>1.0</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
@@ -1990,16 +1952,16 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C4" s="1">
         <v>2.0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
@@ -2007,19 +1969,19 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C5" s="1">
         <v>1.0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6">
@@ -2027,19 +1989,19 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C6" s="1">
         <v>2.0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2048,89 +2010,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="3.25"/>
-    <col customWidth="1" min="3" max="3" width="3.63"/>
-    <col customWidth="1" min="6" max="6" width="17.75"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2154,21 +2033,18 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B2" s="1">
         <v>4.0</v>
@@ -2179,110 +2055,95 @@
       <c r="D2" s="1">
         <v>2.0</v>
       </c>
-      <c r="E2" s="1">
-        <v>2.0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B5" s="1">
         <v>1.0</v>
       </c>
       <c r="C5" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D5" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" ht="26.25" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="A8" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>170</v>
+      <c r="A9" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>